<commit_message>
amend spi2-DI pin to pull up. it needs for SD card output
</commit_message>
<xml_diff>
--- a/parts_List_PIC32MX130_SpeakingClock20170726_02.xlsx
+++ b/parts_List_PIC32MX130_SpeakingClock20170726_02.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="163">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -259,6 +259,9 @@
     <t xml:space="preserve">PIC32MX130F064B</t>
   </si>
   <si>
+    <t xml:space="preserve">IC_SOCKET</t>
+  </si>
+  <si>
     <t xml:space="preserve">IC_SOCKET 28P</t>
   </si>
   <si>
@@ -298,6 +301,9 @@
     <t xml:space="preserve">P-04005</t>
   </si>
   <si>
+    <t xml:space="preserve">TUBE</t>
+  </si>
+  <si>
     <t xml:space="preserve">TUBE 2mmX5mm</t>
   </si>
   <si>
@@ -325,7 +331,7 @@
     <t xml:space="preserve">I-05886</t>
   </si>
   <si>
-    <t xml:space="preserve">TUBE 2mmX10mm</t>
+    <t xml:space="preserve">TUBE 2mmX15mm</t>
   </si>
   <si>
     <t xml:space="preserve">CN1</t>
@@ -340,6 +346,9 @@
     <t xml:space="preserve">P-01306</t>
   </si>
   <si>
+    <t xml:space="preserve">BATTERY_CASE</t>
+  </si>
+  <si>
     <t xml:space="preserve">BATTERY CASE</t>
   </si>
   <si>
@@ -373,16 +382,19 @@
     <t xml:space="preserve">LCD_I2C_AQM1602XA-RN-GBW</t>
   </si>
   <si>
+    <t xml:space="preserve">PIN HEAD 1X4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-03950</t>
+  </si>
+  <si>
     <t xml:space="preserve">AQM1602XA-RN-GBW</t>
   </si>
   <si>
     <t xml:space="preserve">K-08896</t>
   </si>
   <si>
-    <t xml:space="preserve">PIN HEAD 1X4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C-03950</t>
+    <t xml:space="preserve">CONNECTOR_HOUSING</t>
   </si>
   <si>
     <t xml:space="preserve">コネクタハウジング 1X4</t>
@@ -391,6 +403,9 @@
     <t xml:space="preserve">C-12153</t>
   </si>
   <si>
+    <t xml:space="preserve">CONNECTOR</t>
+  </si>
+  <si>
     <t xml:space="preserve">コネクタ端子</t>
   </si>
   <si>
@@ -403,6 +418,9 @@
     <t xml:space="preserve">SP1</t>
   </si>
   <si>
+    <t xml:space="preserve">(SPEAKER)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPEAKER</t>
   </si>
   <si>
@@ -412,27 +430,36 @@
     <t xml:space="preserve">RVR1</t>
   </si>
   <si>
+    <t xml:space="preserve">(10K)</t>
+  </si>
+  <si>
     <t xml:space="preserve">RVR</t>
   </si>
   <si>
+    <t xml:space="preserve">TERMINAL 3P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-01307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VOLUME</t>
+  </si>
+  <si>
     <t xml:space="preserve">VOLUME(10KΩA)</t>
   </si>
   <si>
     <t xml:space="preserve">P00242</t>
   </si>
   <si>
+    <t xml:space="preserve">KNOB</t>
+  </si>
+  <si>
     <t xml:space="preserve">KNOB(ツマミ) 15mm</t>
   </si>
   <si>
     <t xml:space="preserve">P-00253</t>
   </si>
   <si>
-    <t xml:space="preserve">TERMINAL 3P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-01307</t>
-  </si>
-  <si>
     <t xml:space="preserve">WIRE(THIN)]</t>
   </si>
   <si>
@@ -442,28 +469,43 @@
     <t xml:space="preserve">PRINT BOARD</t>
   </si>
   <si>
+    <t xml:space="preserve">ケース</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3mm厚シナベニヤ、切り出し</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JW_CAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ネジ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">基板取り付けネジ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">直径3mmX長さ8mmタッピングネジ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCD取り付けネジ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蓋取り付けネジ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">スピーカ取り付けネジ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">直径3mmX長さ16mmタッピングネジ</t>
+  </si>
+  <si>
     <t xml:space="preserve">(MICRO SD CARD)</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
     <t xml:space="preserve">(BATTERY)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ケース</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3mm厚シナベニヤ、切り出し</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JW_CAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ネジ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">直径3mmタッピングネジ</t>
   </si>
   <si>
     <t xml:space="preserve">total</t>
@@ -510,7 +552,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,7 +562,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -565,7 +613,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -590,6 +638,22 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -602,7 +666,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -667,10 +731,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J80" activeCellId="0" sqref="J80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M61" activeCellId="0" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1159,131 +1223,100 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="J25" s="5" t="n">
-        <f aca="false">H25*I25</f>
-        <v>13</v>
-      </c>
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J26" s="5" t="n">
         <f aca="false">H26*I26</f>
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="3" t="n">
-        <v>220</v>
+        <v>46</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="3" t="n">
-        <v>220</v>
+        <v>47</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I27" s="5" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J27" s="5" t="n">
         <f aca="false">H27*I27</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>220</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>21</v>
@@ -1291,30 +1324,30 @@
       <c r="E29" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>51</v>
+      <c r="F29" s="3" t="n">
+        <v>220</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" s="5" t="n">
         <v>1</v>
       </c>
       <c r="J29" s="5" t="n">
         <f aca="false">H29*I29</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>21</v>
@@ -1323,29 +1356,22 @@
         <v>49</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G30" s="4"/>
-      <c r="H30" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I30" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J30" s="5" t="n">
-        <f aca="false">H30*I30</f>
-        <v>1</v>
-      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="3" t="n">
-        <v>100</v>
+        <v>52</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>21</v>
@@ -1353,30 +1379,30 @@
       <c r="E31" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="3" t="n">
-        <v>100</v>
+      <c r="F31" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I31" s="5" t="n">
         <v>1</v>
       </c>
       <c r="J31" s="5" t="n">
         <f aca="false">H31*I31</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>21</v>
@@ -1385,22 +1411,29 @@
         <v>49</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H32" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" s="5" t="n">
+        <f aca="false">H32*I32</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>100</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>21</v>
@@ -1408,20 +1441,27 @@
       <c r="E33" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>57</v>
+      <c r="F33" s="3" t="n">
+        <v>100</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
+      <c r="H33" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" s="5" t="n">
+        <f aca="false">H33*I33</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>57</v>
@@ -1442,10 +1482,10 @@
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>57</v>
@@ -1466,10 +1506,10 @@
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>57</v>
@@ -1490,10 +1530,10 @@
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>57</v>
@@ -1514,10 +1554,10 @@
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>57</v>
@@ -1536,12 +1576,12 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>57</v>
@@ -1556,83 +1596,83 @@
         <v>57</v>
       </c>
       <c r="G39" s="4"/>
-      <c r="H39" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="I39" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J39" s="5" t="n">
-        <f aca="false">H39*I39</f>
-        <v>8</v>
-      </c>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="A40" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G41" s="4"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="n">
-        <v>31</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G42" s="4"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
+      <c r="H41" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I41" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" s="5" t="n">
+        <f aca="false">H41*I41</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>66</v>
@@ -1653,10 +1693,10 @@
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>66</v>
@@ -1675,15 +1715,15 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>21</v>
@@ -1695,94 +1735,86 @@
         <v>66</v>
       </c>
       <c r="G45" s="4"/>
-      <c r="H45" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I45" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="J45" s="5" t="n">
-        <f aca="false">H45*I45</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H46" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I46" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="J46" s="5" t="n">
-        <f aca="false">H46*I46</f>
-        <v>20</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="G46" s="4"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I47" s="5" t="n">
-        <v>350</v>
+        <v>10</v>
       </c>
       <c r="J47" s="5" t="n">
         <f aca="false">H47*I47</f>
-        <v>350</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
-        <v>37</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="F48" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H48" s="5" t="n">
         <v>1</v>
@@ -1797,288 +1829,294 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>83</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="G49" s="4"/>
       <c r="H49" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I49" s="5" t="n">
-        <v>50</v>
+        <v>350</v>
       </c>
       <c r="J49" s="5" t="n">
         <f aca="false">H49*I49</f>
-        <v>50</v>
+        <v>350</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="B50" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H50" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I50" s="5" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J50" s="5" t="n">
         <f aca="false">H50*I50</f>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H51" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I51" s="5" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J51" s="5" t="n">
         <f aca="false">H51*I51</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="B52" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G52" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="H52" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
+      <c r="I52" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J52" s="5" t="n">
+        <f aca="false">H52*I52</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H53" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I53" s="5" t="n">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="J53" s="5" t="n">
         <f aca="false">H53*I53</f>
-        <v>300</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2"/>
-      <c r="B54" s="3"/>
+      <c r="A54" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="G54" s="4"/>
-      <c r="H54" s="5"/>
+      <c r="H54" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G55" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="H55" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I55" s="5" t="n">
-        <v>25</v>
+        <v>300</v>
       </c>
       <c r="J55" s="5" t="n">
         <f aca="false">H55*I55</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G56" s="4"/>
-      <c r="H56" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G57" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="H57" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I57" s="5" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J57" s="5" t="n">
         <f aca="false">H57*I57</f>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="B58" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>107</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="G58" s="4"/>
       <c r="H58" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I58" s="5" t="n">
-        <v>70</v>
-      </c>
-      <c r="J58" s="5" t="n">
-        <f aca="false">H58*I58</f>
-        <v>70</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H59" s="5" t="n">
         <v>1</v>
@@ -2093,308 +2131,334 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>114</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
       <c r="F60" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="H60" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I60" s="5" t="n">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="J60" s="5" t="n">
         <f aca="false">H60*I60</f>
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H61" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I61" s="5" t="n">
-        <v>550</v>
+        <v>20</v>
       </c>
       <c r="J61" s="5" t="n">
         <f aca="false">H61*I61</f>
-        <v>550</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="F62" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H62" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I62" s="5" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="J62" s="5" t="n">
         <f aca="false">H62*I62</f>
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
-        <v>51</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="F63" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G63" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="H63" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I63" s="5" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J63" s="5" t="n">
         <f aca="false">H63*I63</f>
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
-        <v>52</v>
-      </c>
-      <c r="B64" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G64" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G64" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="H64" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I64" s="5" t="n">
-        <v>5</v>
+        <v>550</v>
       </c>
       <c r="J64" s="5" t="n">
         <f aca="false">H64*I64</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
-        <v>53</v>
-      </c>
-      <c r="B65" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G65" s="4"/>
+      <c r="G65" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="H65" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I65" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J65" s="5" t="n">
+        <f aca="false">H65*I65</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C66" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>127</v>
-      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
       <c r="F66" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H66" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I66" s="5" t="n">
-        <v>300</v>
+        <v>5</v>
       </c>
       <c r="J66" s="5" t="n">
         <f aca="false">H66*I66</f>
-        <v>300</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
-        <v>55</v>
-      </c>
-      <c r="B67" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>105</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="G67" s="4"/>
       <c r="H67" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I67" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H68" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I68" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="J67" s="5" t="n">
-        <f aca="false">H67*I67</f>
+      <c r="J68" s="5" t="n">
+        <f aca="false">H68*I68</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="n">
-        <v>56</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G68" s="4"/>
-      <c r="H68" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>130</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
       <c r="F69" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H69" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I69" s="5" t="n">
-        <v>40</v>
+        <v>300</v>
       </c>
       <c r="J69" s="5" t="n">
         <f aca="false">H69*I69</f>
-        <v>40</v>
+        <v>300</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2"/>
-      <c r="B70" s="3"/>
+      <c r="A70" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>134</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="G70" s="4"/>
       <c r="H70" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I70" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="J70" s="5" t="n">
-        <f aca="false">H70*I70</f>
-        <v>20</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
-        <v>58</v>
-      </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="F71" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H71" s="5" t="n">
         <v>1</v>
@@ -2407,152 +2471,187 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
-        <v>59</v>
-      </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G72" s="4"/>
+        <v>141</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="H72" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-    </row>
-    <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2"/>
-      <c r="B73" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="I72" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="J72" s="5" t="n">
+        <f aca="false">H72*I72</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
+      <c r="F73" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H73" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I73" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="J73" s="5" t="n">
+        <f aca="false">H73*I73</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
         <v>60</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I74" s="5" t="n">
-        <v>300</v>
-      </c>
-      <c r="J74" s="5" t="n">
-        <f aca="false">H74*I74</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-    </row>
-    <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="6"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
         <v>61</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G76" s="4"/>
-      <c r="H76" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
+      <c r="H76" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I76" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="J76" s="5" t="n">
+        <f aca="false">H76*I76</f>
+        <v>300</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="n">
-        <v>62</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="A77" s="2"/>
+      <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="F77" s="3"/>
       <c r="G77" s="4"/>
-      <c r="H77" s="5" t="s">
-        <v>141</v>
-      </c>
+      <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="A78" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
+      <c r="F78" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="G78" s="4"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
+      <c r="H78" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I78" s="5" t="n">
+        <v>285</v>
+      </c>
+      <c r="J78" s="5" t="n">
+        <f aca="false">H78*I78</f>
+        <v>570</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
         <v>63</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="5" t="n">
         <v>2</v>
       </c>
       <c r="I79" s="5" t="n">
-        <v>285</v>
+        <v>5</v>
       </c>
       <c r="J79" s="5" t="n">
         <f aca="false">H79*I79</f>
-        <v>570</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,53 +2659,87 @@
         <v>64</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="5" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I80" s="5" t="n">
         <v>5</v>
       </c>
       <c r="J80" s="5" t="n">
         <f aca="false">H80*I80</f>
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="A81" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
+      <c r="F81" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="G81" s="4"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="5"/>
+      <c r="H81" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I81" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="J81" s="5" t="n">
+        <f aca="false">H81*I81</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="A82" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
+      <c r="F82" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="G82" s="4"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
+      <c r="H82" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I82" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="J82" s="5" t="n">
+        <f aca="false">H82*I82</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2"/>
@@ -2621,42 +2754,84 @@
       <c r="J83" s="5"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2"/>
-      <c r="B84" s="3"/>
+      <c r="A84" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
+      <c r="F84" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="G84" s="4"/>
-      <c r="H84" s="5"/>
+      <c r="H84" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I84" s="5"/>
       <c r="J84" s="5"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2"/>
-      <c r="B85" s="3"/>
+      <c r="A85" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>161</v>
+      </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="G85" s="4"/>
-      <c r="H85" s="5" t="n">
-        <f aca="false">SUM(H11:H84)</f>
-        <v>81</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="J85" s="5" t="n">
-        <f aca="false">SUM(J11:J84)</f>
-        <v>3184</v>
-      </c>
-    </row>
+      <c r="H85" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G87" s="4"/>
+      <c r="H87" s="5" t="n">
+        <f aca="false">SUM(H11:H86)</f>
+        <v>85</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="J87" s="5" t="n">
+        <f aca="false">SUM(J11:J86)</f>
+        <v>3204</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.279861111111111" right="0.3" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.279861111111111" right="0.3" top="0.413194444444444" bottom="0.311111111111111" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>